<commit_message>
send to folder and verify no duplicates
</commit_message>
<xml_diff>
--- a/histogram/result.xlsx
+++ b/histogram/result.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pbermejo/Documents/Master/repos/retinopathy/histogram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{901B21EF-0739-F74C-9347-245334B52FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93FBBC-60FB-064B-BC98-4209A7929934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="32000" windowHeight="17500"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="32000" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="result" sheetId="1" r:id="rId1"/>
@@ -6334,7 +6334,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -6805,7 +6805,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -6848,8 +6848,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6876,8 +6877,11 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -6917,6 +6921,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -7230,12 +7235,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2093"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M2094"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+      <pane ySplit="2" topLeftCell="A2075" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2084" sqref="M2084"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -97204,6 +97209,20 @@
         <v>2090</v>
       </c>
     </row>
+    <row r="2094" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="J2094" s="10">
+        <f>+J2093/$M2093</f>
+        <v>0.76315789473684215</v>
+      </c>
+      <c r="K2094" s="10">
+        <f>+K2093/$M2093</f>
+        <v>0.18516746411483254</v>
+      </c>
+      <c r="L2094" s="10">
+        <f>+L2093/$M2093</f>
+        <v>5.1674641148325359E-2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:L1"/>

</xml_diff>